<commit_message>
Changed to p < 0.01
</commit_message>
<xml_diff>
--- a/data/uw_mapping.xlsx
+++ b/data/uw_mapping.xlsx
@@ -5,34 +5,35 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\nfhs5_analysis\nfhs4 estimates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\external\nfhs-unhealthy-weight\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A67F238-009D-4DDF-AE0A-263F6ECC140C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E679D8A8-1E9C-4335-B53D-41F382219A2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nfhs4 to nfhs5" sheetId="1" r:id="rId1"/>
-    <sheet name="legend" sheetId="2" r:id="rId2"/>
-    <sheet name="nfhs5_state" sheetId="3" r:id="rId3"/>
-    <sheet name="nfhs5_district" sheetId="5" r:id="rId4"/>
-    <sheet name="nfhs4_state" sheetId="6" r:id="rId5"/>
-    <sheet name="nfhs4_district" sheetId="7" r:id="rId6"/>
+    <sheet name="nfhs5_factsheet_map" sheetId="8" r:id="rId2"/>
+    <sheet name="legend" sheetId="2" r:id="rId3"/>
+    <sheet name="nfhs5_state" sheetId="3" r:id="rId4"/>
+    <sheet name="nfhs5_district" sheetId="5" r:id="rId5"/>
+    <sheet name="nfhs4_state" sheetId="6" r:id="rId6"/>
+    <sheet name="nfhs4_district" sheetId="7" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'nfhs4 to nfhs5'!$A$1:$I$708</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">nfhs4_state!$A$1:$B$115</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">nfhs4_state!$A$1:$B$115</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5382" uniqueCount="1374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5493" uniqueCount="1416">
   <si>
     <t>REMARK</t>
   </si>
@@ -4154,6 +4155,132 @@
   </si>
   <si>
     <t>Women who are overweight or obese (BMI = 25.0 kg/m2)14 (%)</t>
+  </si>
+  <si>
+    <t>v024_label</t>
+  </si>
+  <si>
+    <t>factsheet_state</t>
+  </si>
+  <si>
+    <t>v024_nfhs3</t>
+  </si>
+  <si>
+    <t>andaman and nicobar islands</t>
+  </si>
+  <si>
+    <t>andhra pradesh</t>
+  </si>
+  <si>
+    <t>arunachal pradesh</t>
+  </si>
+  <si>
+    <t>assam</t>
+  </si>
+  <si>
+    <t>bihar</t>
+  </si>
+  <si>
+    <t>chandigarh</t>
+  </si>
+  <si>
+    <t>chhattisgarh</t>
+  </si>
+  <si>
+    <t>daman and diu</t>
+  </si>
+  <si>
+    <t>Dadra &amp; Nagar Haveli and Daman &amp; Diu</t>
+  </si>
+  <si>
+    <t>goa</t>
+  </si>
+  <si>
+    <t>gujarat</t>
+  </si>
+  <si>
+    <t>haryana</t>
+  </si>
+  <si>
+    <t>himachal pradesh</t>
+  </si>
+  <si>
+    <t>jammu and kashmir</t>
+  </si>
+  <si>
+    <t>jharkhand</t>
+  </si>
+  <si>
+    <t>karnataka</t>
+  </si>
+  <si>
+    <t>kerala</t>
+  </si>
+  <si>
+    <t>ladakh</t>
+  </si>
+  <si>
+    <t>lakshadweep</t>
+  </si>
+  <si>
+    <t>madhya pradesh</t>
+  </si>
+  <si>
+    <t>maharashtra</t>
+  </si>
+  <si>
+    <t>manipur</t>
+  </si>
+  <si>
+    <t>meghalaya</t>
+  </si>
+  <si>
+    <t>mizoram</t>
+  </si>
+  <si>
+    <t>nagaland</t>
+  </si>
+  <si>
+    <t>delhi</t>
+  </si>
+  <si>
+    <t>odisha</t>
+  </si>
+  <si>
+    <t>orissa</t>
+  </si>
+  <si>
+    <t>puducherry</t>
+  </si>
+  <si>
+    <t>punjab</t>
+  </si>
+  <si>
+    <t>rajasthan</t>
+  </si>
+  <si>
+    <t>sikkim</t>
+  </si>
+  <si>
+    <t>tamil nadu</t>
+  </si>
+  <si>
+    <t>telangana</t>
+  </si>
+  <si>
+    <t>tripura</t>
+  </si>
+  <si>
+    <t>uttar pradesh</t>
+  </si>
+  <si>
+    <t>uttarakhand</t>
+  </si>
+  <si>
+    <t>uttaranchal</t>
+  </si>
+  <si>
+    <t>west bengal</t>
   </si>
 </sst>
 </file>
@@ -5735,7 +5862,7 @@
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A690" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I709" sqref="I709"/>
+      <selection pane="bottomLeft" activeCell="H693" sqref="H693"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24445,6 +24572,428 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B82F205-BE1D-4509-81E9-AF64314EBC5F}">
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1375</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B2" t="s">
+        <v>840</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B4" t="s">
+        <v>432</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B7" t="s">
+        <v>874</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B8" t="s">
+        <v>461</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B12" t="s">
+        <v>505</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B14" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B15" t="s">
+        <v>530</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B16" t="s">
+        <v>201</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B17" t="s">
+        <v>233</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B18" t="s">
+        <v>869</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B19" t="s">
+        <v>873</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B20" t="s">
+        <v>559</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B21" t="s">
+        <v>252</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B22" t="s">
+        <v>308</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B23" t="s">
+        <v>292</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B24" t="s">
+        <v>319</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B25" t="s">
+        <v>329</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B26" t="s">
+        <v>494</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B27" t="s">
+        <v>611</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B28" t="s">
+        <v>671</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B29" t="s">
+        <v>643</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B30" t="s">
+        <v>676</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B31" t="s">
+        <v>342</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B32" t="s">
+        <v>711</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B33" t="s">
+        <v>350</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B34" t="s">
+        <v>394</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B35" t="s">
+        <v>745</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B36" t="s">
+        <v>826</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B37" t="s">
+        <v>408</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7924E170-37AE-4226-9044-712E3AC553CD}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -24534,11 +25083,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F045BF79-003F-470B-8A13-78202BC0A178}">
   <dimension ref="A1:C132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -26004,7 +26555,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4857F10E-FD5A-490D-B1EC-3909C76C2C14}">
   <dimension ref="A1:C105"/>
   <sheetViews>
@@ -27177,7 +27728,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B24FE1F-8B44-4411-ABEB-E4F5D5254ECD}">
   <dimension ref="A1:D115"/>
   <sheetViews>
@@ -28894,7 +29445,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE553DC4-B5B6-40CB-8D09-94AB31CA8142}">
   <dimension ref="A1:C94"/>
   <sheetViews>

</xml_diff>

<commit_message>
Edit in estimates for 4 districts in Uttarakhand
</commit_message>
<xml_diff>
--- a/data/uw_mapping.xlsx
+++ b/data/uw_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\external\nfhs-unhealthy-weight\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E679D8A8-1E9C-4335-B53D-41F382219A2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD7DFAE-54F8-4CAC-854A-D612EBE592FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nfhs4 to nfhs5" sheetId="1" r:id="rId1"/>
@@ -4348,7 +4348,57 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5860,9 +5910,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I708"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A690" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H693" sqref="H693"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A653" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H549" sqref="H549"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24301,7 +24351,7 @@
         <v>34</v>
       </c>
       <c r="B699">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C699" t="s">
         <v>826</v>
@@ -24310,7 +24360,7 @@
         <v>825</v>
       </c>
       <c r="E699" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="F699" t="s">
         <v>825</v>
@@ -24327,7 +24377,7 @@
         <v>34</v>
       </c>
       <c r="B700">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C700" t="s">
         <v>826</v>
@@ -24336,7 +24386,7 @@
         <v>825</v>
       </c>
       <c r="E700" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="F700" t="s">
         <v>825</v>
@@ -24353,7 +24403,7 @@
         <v>34</v>
       </c>
       <c r="B701">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C701" t="s">
         <v>826</v>
@@ -24362,7 +24412,7 @@
         <v>825</v>
       </c>
       <c r="E701" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="F701" t="s">
         <v>825</v>
@@ -24564,7 +24614,13 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I708" xr:uid="{4D44E7C5-82BC-434C-8883-EECA059D5F8A}"/>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B702:B1048576 B1:B700">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B701">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24575,8 +24631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B82F205-BE1D-4509-81E9-AF64314EBC5F}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>